<commit_message>
fixes #13 switch location and events tab so location is first
</commit_message>
<xml_diff>
--- a/inst/app/www/template-bison.xlsx
+++ b/inst/app/www/template-bison.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aylapearson/Applications/poisson/shinybisonpic/inst/app/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A7D54-FA0B-B54A-9CA2-CFCB981DDD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF733B2-97AB-054E-838D-F99DA6930414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32480" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{CBEE4468-5A59-B344-A0B5-6F1F38BE5D82}"/>
   </bookViews>
   <sheets>
-    <sheet name="Events" sheetId="1" r:id="rId1"/>
-    <sheet name="Locations" sheetId="2" r:id="rId2"/>
+    <sheet name="Locations" sheetId="2" r:id="rId1"/>
+    <sheet name="Events" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -579,10 +579,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF429F2-298F-B542-81FC-B30A5252E1A9}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1">
+        <v>57.895690000000002</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-111.67757</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8EEA22-A96D-564A-8B74-E04C99EA5D01}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
+    <sheetView zoomScale="161" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -875,97 +968,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF429F2-298F-B542-81FC-B30A5252E1A9}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="1">
-        <v>57.895690000000002</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-111.67757</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>